<commit_message>
Update data dictionary for TGPs
</commit_message>
<xml_diff>
--- a/data/PQ data/PQCHC_data_plan_dictionary.xlsx
+++ b/data/PQ data/PQCHC_data_plan_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4617e70f33205b2a/Work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4617e70f33205b2a/Documents/GitHub/2021_CensusDataProcessing/data/PQ data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="884" documentId="8_{CE446891-56C3-46A0-B41E-B43D6D107E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6AF0FEC-7DFB-4B97-B319-248951FEEA37}"/>
+  <xr:revisionPtr revIDLastSave="887" documentId="8_{CE446891-56C3-46A0-B41E-B43D6D107E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A209FC1-7C0A-42EF-B718-DAC0071B261B}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="105" windowWidth="14025" windowHeight="15510" firstSheet="1" activeTab="1" xr2:uid="{78EF0FB6-9AB1-4EDB-B7C7-CDF5A0E6492F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="2" xr2:uid="{78EF0FB6-9AB1-4EDB-B7C7-CDF5A0E6492F}"/>
   </bookViews>
   <sheets>
     <sheet name="Selected Data IDs" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={269D91A4-75DC-4F9F-A523-3EC36B87651D}</author>
-    <author>tc={9009B201-6F22-4614-8615-6EAB65F7AC31}</author>
     <author>tc={B09EF3BD-E05E-4CB8-A10B-7AB75E5ACD78}</author>
   </authors>
   <commentList>
@@ -109,17 +108,7 @@
     This data dictionary table is to be used for the TGPs (immigrants, seniors 65+, youth 15-64, etc.)</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{9009B201-6F22-4614-8615-6EAB65F7AC31}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Percentage 1 = percentage that is already calculated in the Census profile, so the denominator is ONE
-Percentage 2 = percentage that we would need to calculate using a denominator that has a Data_ID
-</t>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{B09EF3BD-E05E-4CB8-A10B-7AB75E5ACD78}">
+    <comment ref="A5" authorId="1" shapeId="0" xr:uid="{B09EF3BD-E05E-4CB8-A10B-7AB75E5ACD78}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="399">
   <si>
     <t>Data_ID</t>
   </si>
@@ -1314,13 +1303,28 @@
   </si>
   <si>
     <t>% of pop that are seniors age 65+</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>Numerator</t>
+  </si>
+  <si>
+    <t>Denominator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1712,11 +1716,6 @@
   <threadedComment ref="A1" dT="2023-09-01T18:51:04.49" personId="{361E46C3-40A8-4886-8719-7FA472AE0D59}" id="{269D91A4-75DC-4F9F-A523-3EC36B87651D}">
     <text>This data dictionary table is to be used for the TGPs (immigrants, seniors 65+, youth 15-64, etc.)</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2023-09-01T13:58:25.44" personId="{361E46C3-40A8-4886-8719-7FA472AE0D59}" id="{9009B201-6F22-4614-8615-6EAB65F7AC31}">
-    <text xml:space="preserve">Percentage 1 = percentage that is already calculated in the Census profile, so the denominator is ONE
-Percentage 2 = percentage that we would need to calculate using a denominator that has a Data_ID
-</text>
-  </threadedComment>
   <threadedComment ref="A5" dT="2023-09-01T13:54:58.38" personId="{361E46C3-40A8-4886-8719-7FA472AE0D59}" id="{B09EF3BD-E05E-4CB8-A10B-7AB75E5ACD78}">
     <text>Using among recipients instead of among households, so that we can give comparisons between the general pop and TGPs like immigrants and seniors</text>
   </threadedComment>
@@ -1731,18 +1730,18 @@
       <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" customWidth="1"/>
+    <col min="7" max="7" width="20.59765625" customWidth="1"/>
     <col min="8" max="8" width="60" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1942,11 +1941,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1970,7 +1969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1978,7 +1977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -2010,7 +2009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2050,7 +2049,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2074,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -2082,7 +2081,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2098,7 +2097,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2106,7 +2105,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -2130,7 +2129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>100</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -2162,7 +2161,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -2178,7 +2177,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>108</v>
       </c>
@@ -2186,7 +2185,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -2194,7 +2193,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -2202,7 +2201,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -2218,7 +2217,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>118</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>120</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2258,7 +2257,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -2274,7 +2273,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>132</v>
       </c>
@@ -2282,7 +2281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>138</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -2314,7 +2313,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>142</v>
       </c>
@@ -2322,7 +2321,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>144</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>146</v>
       </c>
@@ -2338,7 +2337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>148</v>
       </c>
@@ -2346,7 +2345,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>150</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>152</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>154</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>156</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>158</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>160</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>164</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>166</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>168</v>
       </c>
@@ -2426,7 +2425,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>170</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>172</v>
       </c>
@@ -2442,7 +2441,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>174</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>176</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>180</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>182</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>184</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>186</v>
       </c>
@@ -2498,7 +2497,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -2506,7 +2505,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>190</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>192</v>
       </c>
@@ -2522,7 +2521,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>194</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>196</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -2546,7 +2545,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>200</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>202</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>204</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>206</v>
       </c>
@@ -2578,7 +2577,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>208</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>210</v>
       </c>
@@ -2594,7 +2593,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>212</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>214</v>
       </c>
@@ -2610,7 +2609,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>216</v>
       </c>
@@ -2618,7 +2617,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>218</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>220</v>
       </c>
@@ -2634,7 +2633,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>222</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>224</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>226</v>
       </c>
@@ -2658,7 +2657,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>228</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>230</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>232</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>233</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>234</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>235</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>236</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>237</v>
       </c>
@@ -2722,7 +2721,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>238</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>239</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>240</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>242</v>
       </c>
@@ -2754,7 +2753,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>244</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>246</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>250</v>
       </c>
@@ -2786,7 +2785,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>252</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>253</v>
       </c>
@@ -2802,7 +2801,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>254</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>256</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>258</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
         <v>260</v>
       </c>
@@ -2834,7 +2833,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>262</v>
       </c>
@@ -2842,7 +2841,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>264</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>266</v>
       </c>
@@ -2858,7 +2857,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>268</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>270</v>
       </c>
@@ -2874,7 +2873,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -2882,7 +2881,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>274</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>276</v>
       </c>
@@ -2910,20 +2909,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F66F677-454E-4559-B256-926A3CFA8762}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+    <sheetView topLeftCell="B58" workbookViewId="0">
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -2940,7 +2939,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>286</v>
       </c>
@@ -2974,7 +2973,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>288</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -3008,7 +3007,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>298</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>299</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>300</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -3144,7 +3143,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>302</v>
       </c>
@@ -3161,7 +3160,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>303</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>305</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>307</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>309</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>311</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>313</v>
       </c>
@@ -3280,7 +3279,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -3297,7 +3296,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -3314,7 +3313,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>316</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>317</v>
       </c>
@@ -3348,7 +3347,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>318</v>
       </c>
@@ -3365,7 +3364,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>319</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>320</v>
       </c>
@@ -3399,7 +3398,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>321</v>
       </c>
@@ -3416,7 +3415,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>322</v>
       </c>
@@ -3433,7 +3432,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>323</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>324</v>
       </c>
@@ -3467,7 +3466,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>325</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>326</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>327</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>328</v>
       </c>
@@ -3535,7 +3534,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>329</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>330</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>331</v>
       </c>
@@ -3586,7 +3585,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>332</v>
       </c>
@@ -3603,7 +3602,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>333</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>334</v>
       </c>
@@ -3637,7 +3636,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>335</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>336</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>337</v>
       </c>
@@ -3688,7 +3687,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>338</v>
       </c>
@@ -3705,7 +3704,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>339</v>
       </c>
@@ -3722,7 +3721,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>340</v>
       </c>
@@ -3739,7 +3738,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>341</v>
       </c>
@@ -3756,7 +3755,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>342</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>343</v>
       </c>
@@ -3790,7 +3789,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>344</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>345</v>
       </c>
@@ -3824,7 +3823,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -3841,7 +3840,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>347</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>348</v>
       </c>
@@ -3875,7 +3874,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>349</v>
       </c>
@@ -3892,7 +3891,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>350</v>
       </c>
@@ -3909,7 +3908,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>351</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>149</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -3960,7 +3959,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>352</v>
       </c>
@@ -3977,7 +3976,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>353</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>355</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>356</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>357</v>
       </c>
@@ -4045,7 +4044,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>358</v>
       </c>
@@ -4062,7 +4061,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>359</v>
       </c>
@@ -4079,7 +4078,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>362</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -4130,7 +4129,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>364</v>
       </c>
@@ -4147,7 +4146,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>365</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>366</v>
       </c>
@@ -4181,7 +4180,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>367</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>368</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>369</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>370</v>
       </c>
@@ -4249,7 +4248,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>371</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>372</v>
       </c>
@@ -4280,7 +4279,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>373</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>374</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>375</v>
       </c>
@@ -4328,7 +4327,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>376</v>
       </c>
@@ -4345,7 +4344,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>377</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>378</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -4396,7 +4395,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>380</v>
       </c>
@@ -4423,28 +4422,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCA43BB-30E2-401A-9C83-B0FADBF7E7D9}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.73046875" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>397</v>
       </c>
       <c r="C1" t="s">
-        <v>280</v>
+        <v>398</v>
       </c>
       <c r="D1" t="s">
         <v>281</v>
@@ -4453,114 +4452,114 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>392</v>
       </c>
       <c r="B2">
-        <v>1758</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>283</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>381</v>
       </c>
-      <c r="B3">
+      <c r="B8">
         <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B4">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>283</v>
-      </c>
-      <c r="D4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B5">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D5" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>314</v>
-      </c>
-      <c r="B6">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B7">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E7" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>316</v>
-      </c>
-      <c r="B8">
-        <v>146</v>
       </c>
       <c r="C8" t="s">
         <v>283</v>
@@ -4572,63 +4571,63 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B9">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>283</v>
       </c>
       <c r="D9" t="s">
-        <v>289</v>
+        <v>394</v>
       </c>
       <c r="E9" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>382</v>
       </c>
       <c r="B10">
-        <v>159</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>283</v>
       </c>
       <c r="D10" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="B11">
-        <v>171</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>283</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>394</v>
       </c>
       <c r="E11" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B12">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
         <v>283</v>
@@ -4640,92 +4639,92 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>383</v>
+        <v>315</v>
       </c>
       <c r="B13">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>283</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>394</v>
       </c>
       <c r="E13" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>384</v>
+        <v>316</v>
       </c>
       <c r="B14">
-        <v>42</v>
-      </c>
-      <c r="C14">
-        <v>34</v>
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>283</v>
       </c>
       <c r="D14" t="s">
-        <v>292</v>
+        <v>394</v>
       </c>
       <c r="E14" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>385</v>
+        <v>317</v>
       </c>
       <c r="B15">
-        <v>1848</v>
-      </c>
-      <c r="C15">
-        <v>1847</v>
+        <v>159</v>
+      </c>
+      <c r="C15" t="s">
+        <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>378</v>
+        <v>327</v>
       </c>
       <c r="B16">
-        <v>1849</v>
-      </c>
-      <c r="C16">
-        <v>1847</v>
+        <v>171</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
       </c>
       <c r="D16" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E16" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>386</v>
+        <v>328</v>
       </c>
       <c r="B17">
-        <v>1853</v>
+        <v>171</v>
       </c>
       <c r="C17">
-        <v>1850</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
         <v>292</v>
       </c>
       <c r="E17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>387</v>
       </c>
@@ -4742,7 +4741,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>388</v>
       </c>
@@ -4759,63 +4758,63 @@
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>353</v>
-      </c>
-      <c r="B20" t="s">
-        <v>389</v>
-      </c>
-      <c r="C20" t="s">
-        <v>283</v>
+        <v>295</v>
+      </c>
+      <c r="B20">
+        <v>1234</v>
+      </c>
+      <c r="C20">
+        <v>1233</v>
       </c>
       <c r="D20" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E20" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>355</v>
-      </c>
-      <c r="B21" t="s">
-        <v>389</v>
-      </c>
-      <c r="C21">
-        <v>566</v>
+        <v>346</v>
+      </c>
+      <c r="B21">
+        <v>1234</v>
+      </c>
+      <c r="C21" t="s">
+        <v>283</v>
       </c>
       <c r="D21" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E21" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>390</v>
+        <v>297</v>
       </c>
       <c r="B22">
-        <v>2375</v>
+        <v>1236</v>
       </c>
       <c r="C22">
-        <v>2370</v>
+        <v>1233</v>
       </c>
       <c r="D22" t="s">
         <v>292</v>
       </c>
       <c r="E22" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="B23">
-        <v>2353</v>
+        <v>1236</v>
       </c>
       <c r="C23" t="s">
         <v>283</v>
@@ -4824,32 +4823,32 @@
         <v>284</v>
       </c>
       <c r="E23" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>371</v>
+        <v>298</v>
       </c>
       <c r="B24">
-        <v>2353</v>
+        <v>1237</v>
       </c>
       <c r="C24">
-        <v>2352</v>
+        <v>1233</v>
       </c>
       <c r="D24" t="s">
         <v>292</v>
       </c>
       <c r="E24" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="B25">
-        <v>2355</v>
+        <v>1237</v>
       </c>
       <c r="C25" t="s">
         <v>283</v>
@@ -4858,32 +4857,32 @@
         <v>284</v>
       </c>
       <c r="E25" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>299</v>
       </c>
       <c r="B26">
-        <v>2355</v>
+        <v>1238</v>
       </c>
       <c r="C26">
-        <v>2352</v>
+        <v>1233</v>
       </c>
       <c r="D26" t="s">
         <v>292</v>
       </c>
       <c r="E26" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B27">
-        <v>32</v>
+        <v>1238</v>
       </c>
       <c r="C27" t="s">
         <v>283</v>
@@ -4892,32 +4891,32 @@
         <v>284</v>
       </c>
       <c r="E27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="B28">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>283</v>
+        <v>1429</v>
+      </c>
+      <c r="C28">
+        <v>1428</v>
       </c>
       <c r="D28" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E28" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>286</v>
-      </c>
-      <c r="B29" t="s">
-        <v>287</v>
+        <v>380</v>
+      </c>
+      <c r="B29">
+        <v>1429</v>
       </c>
       <c r="C29" t="s">
         <v>283</v>
@@ -4929,165 +4928,165 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>391</v>
-      </c>
-      <c r="B30" t="s">
-        <v>287</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>1758</v>
+      </c>
+      <c r="C30" t="s">
+        <v>283</v>
       </c>
       <c r="D30" t="s">
+        <v>289</v>
+      </c>
+      <c r="E30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>385</v>
+      </c>
+      <c r="B31">
+        <v>1848</v>
+      </c>
+      <c r="C31">
+        <v>1847</v>
+      </c>
+      <c r="D31" t="s">
         <v>292</v>
       </c>
-      <c r="E30" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>392</v>
-      </c>
-      <c r="B31">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>283</v>
-      </c>
-      <c r="D31" t="s">
-        <v>284</v>
-      </c>
       <c r="E31" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>1849</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>1847</v>
       </c>
       <c r="D32" t="s">
         <v>292</v>
       </c>
       <c r="E32" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
       <c r="B33">
-        <v>1234</v>
+        <v>1853</v>
       </c>
       <c r="C33">
-        <v>1233</v>
+        <v>1850</v>
       </c>
       <c r="D33" t="s">
         <v>292</v>
       </c>
       <c r="E33" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>370</v>
       </c>
       <c r="B34">
-        <v>1236</v>
-      </c>
-      <c r="C34">
-        <v>1233</v>
+        <v>2353</v>
+      </c>
+      <c r="C34" t="s">
+        <v>283</v>
       </c>
       <c r="D34" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E34" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>298</v>
+        <v>371</v>
       </c>
       <c r="B35">
-        <v>1237</v>
+        <v>2353</v>
       </c>
       <c r="C35">
-        <v>1233</v>
+        <v>2352</v>
       </c>
       <c r="D35" t="s">
         <v>292</v>
       </c>
       <c r="E35" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>299</v>
+        <v>372</v>
       </c>
       <c r="B36">
-        <v>1238</v>
-      </c>
-      <c r="C36">
-        <v>1233</v>
+        <v>2355</v>
+      </c>
+      <c r="C36" t="s">
+        <v>283</v>
       </c>
       <c r="D36" t="s">
+        <v>284</v>
+      </c>
+      <c r="E36" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>373</v>
+      </c>
+      <c r="B37">
+        <v>2355</v>
+      </c>
+      <c r="C37">
+        <v>2352</v>
+      </c>
+      <c r="D37" t="s">
         <v>292</v>
       </c>
-      <c r="E36" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>346</v>
-      </c>
-      <c r="B37">
-        <v>1234</v>
-      </c>
-      <c r="C37" t="s">
-        <v>283</v>
-      </c>
-      <c r="D37" t="s">
-        <v>284</v>
-      </c>
       <c r="E37" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="B38">
-        <v>1236</v>
-      </c>
-      <c r="C38" t="s">
-        <v>283</v>
+        <v>2375</v>
+      </c>
+      <c r="C38">
+        <v>2370</v>
       </c>
       <c r="D38" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E38" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>348</v>
-      </c>
-      <c r="B39">
-        <v>1237</v>
+        <v>353</v>
+      </c>
+      <c r="B39" t="s">
+        <v>389</v>
       </c>
       <c r="C39" t="s">
         <v>283</v>
@@ -5096,55 +5095,55 @@
         <v>284</v>
       </c>
       <c r="E39" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>349</v>
-      </c>
-      <c r="B40">
-        <v>1238</v>
-      </c>
-      <c r="C40" t="s">
-        <v>283</v>
+        <v>355</v>
+      </c>
+      <c r="B40" t="s">
+        <v>389</v>
+      </c>
+      <c r="C40">
+        <v>566</v>
       </c>
       <c r="D40" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E40" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>300</v>
-      </c>
-      <c r="B41">
-        <v>1429</v>
-      </c>
-      <c r="C41">
-        <v>1428</v>
+        <v>286</v>
+      </c>
+      <c r="B41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C41" t="s">
+        <v>283</v>
       </c>
       <c r="D41" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E41" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>380</v>
-      </c>
-      <c r="B42">
-        <v>1429</v>
-      </c>
-      <c r="C42" t="s">
-        <v>283</v>
+        <v>391</v>
+      </c>
+      <c r="B42" t="s">
+        <v>287</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E42" t="s">
         <v>285</v>
@@ -5157,27 +5156,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="fb824588-f366-4339-a49f-7eff4c1b42d9" xsi:nil="true"/>
-    <Lastedited xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EE7EE696B873A41BEAC8257087746C3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ef739d34c3db00d072e7fd3175074e46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="124915e9-a20b-402d-bc33-fbef48c2c5dc" xmlns:ns3="fb824588-f366-4339-a49f-7eff4c1b42d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="757988175f1c3dcec2a34a679bb9ba6b" ns2:_="" ns3:_="">
     <xsd:import namespace="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
@@ -5426,14 +5404,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fb824588-f366-4339-a49f-7eff4c1b42d9" xsi:nil="true"/>
+    <Lastedited xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E287C00-EF61-4880-92D0-FFAAD3E8160D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26D92BA1-1FBA-4034-8268-15AF08A759B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
+    <ds:schemaRef ds:uri="fb824588-f366-4339-a49f-7eff4c1b42d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D959687F-11C2-44F9-9F78-B13D5B9F6472}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D959687F-11C2-44F9-9F78-B13D5B9F6472}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26D92BA1-1FBA-4034-8268-15AF08A759B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E287C00-EF61-4880-92D0-FFAAD3E8160D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb824588-f366-4339-a49f-7eff4c1b42d9"/>
+    <ds:schemaRef ds:uri="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>